<commit_message>
Data file for "data_input_pandas.ipynb notebook"
</commit_message>
<xml_diff>
--- a/Data_Input_Notebook.xlsx
+++ b/Data_Input_Notebook.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>Childname</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -433,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -447,42 +459,36 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1001</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -490,34 +496,48 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>1003</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>1004</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -587,7 +607,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -595,7 +615,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -605,8 +625,11 @@
       <c r="C1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -616,8 +639,11 @@
       <c r="C2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -627,16 +653,25 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1002</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1002</v>
       </c>
@@ -646,8 +681,11 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1004</v>
       </c>
@@ -656,6 +694,9 @@
       </c>
       <c r="C6" t="s">
         <v>20</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>